<commit_message>
updates metric names for metrics 5d-5g to reflect the latest names and adds new metric 5h to the template
</commit_message>
<xml_diff>
--- a/data/templates/tlhc_datasheet_template.xlsx
+++ b/data/templates/tlhc_datasheet_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{BEE1AA2F-A70D-4E5F-925E-8A012C13EAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49A640B7-2A44-41BA-89A7-298D53FBB021}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{BEE1AA2F-A70D-4E5F-925E-8A012C13EAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD433E08-6D28-49D1-B3CD-A0069C285B81}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="585" windowWidth="17655" windowHeight="20130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="13785" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Numerator</t>
   </si>
@@ -211,15 +211,6 @@
     <t>Number of participants who did not attend their initial LDCT scan appointment</t>
   </si>
   <si>
-    <t>Number of participants who have had a 3 month follow up LDCT scan performed</t>
-  </si>
-  <si>
-    <t>Number of participants who have had a 12 month follow up LDCT scan performed</t>
-  </si>
-  <si>
-    <t>Number of participants who have had a 24 month follow up LDCT scan performed</t>
-  </si>
-  <si>
     <t>Number of participants with a Lung Cancer diagnosed at stage 1</t>
   </si>
   <si>
@@ -316,9 +307,6 @@
     <t>5g</t>
   </si>
   <si>
-    <t>Number of participants who have had a 48 month surveillance LDCT scan performed</t>
-  </si>
-  <si>
     <t>Number of participants with incidental findings - Pleural effusions/thickening - J91X; J92; J920; J929</t>
   </si>
   <si>
@@ -332,6 +320,24 @@
   </si>
   <si>
     <t>Number of participants who were offered or referred to a smoking cessation course</t>
+  </si>
+  <si>
+    <t>Number of participants who have had a 3 month follow up nodule surveillance LDCT scan performed</t>
+  </si>
+  <si>
+    <t>Number of participants who have had a 12 month follow up nodule surveillance LDCT scan performed</t>
+  </si>
+  <si>
+    <t>Number of participants who have had a 24 month incident screening round LDCT scan performed</t>
+  </si>
+  <si>
+    <t>Number of participants who have had a 48 month incident screening round LDCT scan performed</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>Number of participants who have had a nodule surveillance LDCT scan performed from a 24 months incident screening round scan onwards</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A367F8-4EAE-4C48-B5E2-7F5700B2188B}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +746,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -751,7 +757,7 @@
         <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -762,7 +768,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -784,7 +790,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -795,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -806,7 +812,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -817,7 +823,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -825,7 +831,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>46</v>
@@ -872,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -883,7 +889,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -894,7 +900,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -902,10 +908,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -913,10 +919,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -924,10 +930,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -935,10 +941,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -946,10 +952,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -957,32 +963,32 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>7</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -990,10 +996,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1001,10 +1007,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1012,10 +1018,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -1023,10 +1029,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1034,10 +1040,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1045,10 +1051,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1056,10 +1062,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -1067,10 +1073,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -1078,10 +1084,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1089,10 +1095,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -1100,10 +1106,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1111,10 +1117,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
@@ -1122,10 +1128,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -1133,10 +1139,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
@@ -1144,10 +1150,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -1155,10 +1161,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -1166,10 +1172,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
@@ -1177,10 +1183,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
@@ -1188,10 +1194,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
@@ -1199,10 +1205,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
@@ -1210,10 +1216,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1">
         <v>0</v>
@@ -1221,21 +1227,21 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>9</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
@@ -1243,10 +1249,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
@@ -1254,10 +1260,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
@@ -1265,10 +1271,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
@@ -1276,10 +1282,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -1287,12 +1293,23 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
+        <v>13</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
         <v>14</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="1">
+      <c r="B53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds metric 5h and tweaks to layout
</commit_message>
<xml_diff>
--- a/data/templates/tlhc_datasheet_template.xlsx
+++ b/data/templates/tlhc_datasheet_template.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{BEE1AA2F-A70D-4E5F-925E-8A012C13EAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD433E08-6D28-49D1-B3CD-A0069C285B81}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3045" windowWidth="13785" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25470" yWindow="3315" windowWidth="25365" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -720,7 +720,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>